<commit_message>
Made separate graph pages
</commit_message>
<xml_diff>
--- a/Final Paper/Comparison Table.xlsx
+++ b/Final Paper/Comparison Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c07c9239cf8ef362/4th Year Sem2/EG4012/Matlab GUI Thesis/Matlab-GUI-Thesis/Final Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="5317D6875B4462F98844B3014096D562A4FC8AAC" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{192F9621-C943-44C6-B717-43DA50ED0B3E}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="5317D6875B4462F98844B3014096D562A4FC8AAC" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{4C15C5F7-28AC-481E-81B2-4C2FC6DE9897}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2307,8 +2307,8 @@
   </sheetPr>
   <dimension ref="A1:Q136"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3378,7 +3378,9 @@
       <c r="A40" s="108" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="118"/>
+      <c r="B40" s="118">
+        <v>19.2</v>
+      </c>
       <c r="C40" s="118"/>
       <c r="D40" s="118"/>
       <c r="E40" s="118"/>
@@ -3389,7 +3391,9 @@
       <c r="A41" s="108" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="118"/>
+      <c r="B41" s="118">
+        <v>24.68</v>
+      </c>
       <c r="C41" s="118"/>
       <c r="D41" s="118"/>
       <c r="E41" s="118"/>
@@ -3400,7 +3404,9 @@
       <c r="A42" s="108" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="118"/>
+      <c r="B42" s="118">
+        <v>10</v>
+      </c>
       <c r="C42" s="118"/>
       <c r="D42" s="118"/>
       <c r="E42" s="118"/>
@@ -3411,7 +3417,9 @@
       <c r="A43" s="108" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="118"/>
+      <c r="B43" s="118">
+        <v>6.45</v>
+      </c>
       <c r="C43" s="118"/>
       <c r="D43" s="118"/>
       <c r="E43" s="118"/>
@@ -3422,7 +3430,9 @@
       <c r="A44" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="118"/>
+      <c r="B44" s="118">
+        <v>5.3259999999999996</v>
+      </c>
       <c r="C44" s="118"/>
       <c r="D44" s="118"/>
       <c r="E44" s="118"/>
@@ -3433,7 +3443,9 @@
       <c r="A45" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="118"/>
+      <c r="B45" s="118">
+        <v>0.29599999999999999</v>
+      </c>
       <c r="C45" s="118"/>
       <c r="D45" s="118"/>
       <c r="E45" s="118"/>
@@ -3444,7 +3456,9 @@
       <c r="A46" s="108" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="118"/>
+      <c r="B46" s="118">
+        <v>0.499</v>
+      </c>
       <c r="C46" s="118"/>
       <c r="D46" s="118"/>
       <c r="E46" s="118"/>
@@ -3455,7 +3469,9 @@
       <c r="A47" s="108" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="118"/>
+      <c r="B47" s="118">
+        <v>5.556</v>
+      </c>
       <c r="C47" s="118"/>
       <c r="D47" s="118"/>
       <c r="E47" s="118"/>

</xml_diff>